<commit_message>
Upload excel files with prices
</commit_message>
<xml_diff>
--- a/bots/crawl_ch/output/bread_coop_2022-06-21.xlsx
+++ b/bots/crawl_ch/output/bread_coop_2022-06-21.xlsx
@@ -585,7 +585,7 @@
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1505,7 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3563,7 +3563,7 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3637,7 +3637,7 @@
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3867,7 @@
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4175,7 +4175,7 @@
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4249,7 +4249,7 @@
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4315,7 +4315,7 @@
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4467,7 +4467,7 @@
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4541,7 +4541,7 @@
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4619,7 +4619,7 @@
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4693,7 +4693,7 @@
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4923,7 +4923,7 @@
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5151,7 +5151,7 @@
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5299,7 +5299,7 @@
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5611,7 +5611,7 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5763,7 +5763,7 @@
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5915,7 +5915,7 @@
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -5993,7 +5993,7 @@
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6149,7 +6149,7 @@
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6379,7 +6379,7 @@
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6453,7 +6453,7 @@
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6531,7 +6531,7 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6609,7 +6609,7 @@
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6687,7 +6687,7 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6839,7 +6839,7 @@
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6913,7 +6913,7 @@
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -6991,7 +6991,7 @@
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7065,7 +7065,7 @@
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7139,7 +7139,7 @@
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7295,7 +7295,7 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7369,7 +7369,7 @@
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7447,7 +7447,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7681,7 +7681,7 @@
       </c>
       <c r="P95" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7759,7 +7759,7 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7833,7 +7833,7 @@
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7907,7 +7907,7 @@
       <c r="O98" t="inlineStr"/>
       <c r="P98" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="P99" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8055,7 +8055,7 @@
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8129,7 +8129,7 @@
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8207,7 +8207,7 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8281,7 +8281,7 @@
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8355,7 +8355,7 @@
       <c r="O104" t="inlineStr"/>
       <c r="P104" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
       <c r="O105" t="inlineStr"/>
       <c r="P105" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8507,7 +8507,7 @@
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8581,7 +8581,7 @@
       <c r="O107" t="inlineStr"/>
       <c r="P107" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8659,7 +8659,7 @@
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8737,7 +8737,7 @@
       </c>
       <c r="P109" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8893,7 +8893,7 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -8967,7 +8967,7 @@
       <c r="O112" t="inlineStr"/>
       <c r="P112" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9041,7 +9041,7 @@
       <c r="O113" t="inlineStr"/>
       <c r="P113" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9119,7 +9119,7 @@
       </c>
       <c r="P114" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9197,7 +9197,7 @@
       </c>
       <c r="P115" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9275,7 +9275,7 @@
       </c>
       <c r="P116" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9353,7 +9353,7 @@
       </c>
       <c r="P117" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="P118" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9505,7 +9505,7 @@
       <c r="O119" t="inlineStr"/>
       <c r="P119" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9583,7 +9583,7 @@
       </c>
       <c r="P120" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9661,7 +9661,7 @@
       </c>
       <c r="P121" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9735,7 +9735,7 @@
       <c r="O122" t="inlineStr"/>
       <c r="P122" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9809,7 +9809,7 @@
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9883,7 +9883,7 @@
       <c r="O124" t="inlineStr"/>
       <c r="P124" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="P125" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10035,7 +10035,7 @@
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10113,7 +10113,7 @@
       </c>
       <c r="P127" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10187,7 +10187,7 @@
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10265,7 +10265,7 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10339,7 +10339,7 @@
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10413,7 +10413,7 @@
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10487,7 +10487,7 @@
       <c r="O132" t="inlineStr"/>
       <c r="P132" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="P133" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10639,7 +10639,7 @@
       <c r="O134" t="inlineStr"/>
       <c r="P134" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10713,7 +10713,7 @@
       <c r="O135" t="inlineStr"/>
       <c r="P135" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10791,7 +10791,7 @@
       </c>
       <c r="P136" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10865,7 +10865,7 @@
       <c r="O137" t="inlineStr"/>
       <c r="P137" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -10943,7 +10943,7 @@
       </c>
       <c r="P138" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11017,7 +11017,7 @@
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11091,7 +11091,7 @@
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="P141" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11247,7 +11247,7 @@
       </c>
       <c r="P142" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11325,7 +11325,7 @@
       </c>
       <c r="P143" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11403,7 +11403,7 @@
       </c>
       <c r="P144" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11481,7 +11481,7 @@
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11555,7 +11555,7 @@
       <c r="O146" t="inlineStr"/>
       <c r="P146" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="P147" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11785,7 +11785,7 @@
       </c>
       <c r="P149" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11857,7 +11857,7 @@
       <c r="O150" t="inlineStr"/>
       <c r="P150" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -11931,7 +11931,7 @@
       <c r="O151" t="inlineStr"/>
       <c r="P151" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12005,7 +12005,7 @@
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12081,7 +12081,7 @@
       </c>
       <c r="P153" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12159,7 +12159,7 @@
       </c>
       <c r="P154" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12233,7 +12233,7 @@
       <c r="O155" t="inlineStr"/>
       <c r="P155" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12307,7 +12307,7 @@
       <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12381,7 +12381,7 @@
       <c r="O157" t="inlineStr"/>
       <c r="P157" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12455,7 +12455,7 @@
       <c r="O158" t="inlineStr"/>
       <c r="P158" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12533,7 +12533,7 @@
       </c>
       <c r="P159" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12607,7 +12607,7 @@
       <c r="O160" t="inlineStr"/>
       <c r="P160" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12681,7 +12681,7 @@
       <c r="O161" t="inlineStr"/>
       <c r="P161" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12755,7 +12755,7 @@
       <c r="O162" t="inlineStr"/>
       <c r="P162" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12829,7 +12829,7 @@
       <c r="O163" t="inlineStr"/>
       <c r="P163" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12907,7 +12907,7 @@
       </c>
       <c r="P164" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -12981,7 +12981,7 @@
       <c r="O165" t="inlineStr"/>
       <c r="P165" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13055,7 +13055,7 @@
       <c r="O166" t="inlineStr"/>
       <c r="P166" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13133,7 +13133,7 @@
       </c>
       <c r="P167" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13207,7 +13207,7 @@
       <c r="O168" t="inlineStr"/>
       <c r="P168" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13281,7 +13281,7 @@
       <c r="O169" t="inlineStr"/>
       <c r="P169" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13359,7 +13359,7 @@
       </c>
       <c r="P170" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13435,7 +13435,7 @@
       </c>
       <c r="P171" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13513,7 +13513,7 @@
       </c>
       <c r="P172" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13587,7 +13587,7 @@
       <c r="O173" t="inlineStr"/>
       <c r="P173" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13661,7 +13661,7 @@
       <c r="O174" t="inlineStr"/>
       <c r="P174" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13739,7 +13739,7 @@
       </c>
       <c r="P175" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13817,7 +13817,7 @@
       </c>
       <c r="P176" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13895,7 +13895,7 @@
       </c>
       <c r="P177" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -13969,7 +13969,7 @@
       <c r="O178" t="inlineStr"/>
       <c r="P178" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14047,7 +14047,7 @@
       </c>
       <c r="P179" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14121,7 +14121,7 @@
       <c r="O180" t="inlineStr"/>
       <c r="P180" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14199,7 +14199,7 @@
       </c>
       <c r="P181" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14277,7 +14277,7 @@
       </c>
       <c r="P182" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14355,7 +14355,7 @@
       </c>
       <c r="P183" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14429,7 +14429,7 @@
       <c r="O184" t="inlineStr"/>
       <c r="P184" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14503,7 +14503,7 @@
       <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14577,7 +14577,7 @@
       <c r="O186" t="inlineStr"/>
       <c r="P186" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14651,7 +14651,7 @@
       <c r="O187" t="inlineStr"/>
       <c r="P187" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14729,7 +14729,7 @@
       </c>
       <c r="P188" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14803,7 +14803,7 @@
       <c r="O189" t="inlineStr"/>
       <c r="P189" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14877,7 +14877,7 @@
       <c r="O190" t="inlineStr"/>
       <c r="P190" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -14951,7 +14951,7 @@
       <c r="O191" t="inlineStr"/>
       <c r="P191" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15029,7 +15029,7 @@
       </c>
       <c r="P192" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15103,7 +15103,7 @@
       <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15177,7 +15177,7 @@
       <c r="O194" t="inlineStr"/>
       <c r="P194" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15255,7 +15255,7 @@
       </c>
       <c r="P195" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15333,7 +15333,7 @@
       </c>
       <c r="P196" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15411,7 +15411,7 @@
       </c>
       <c r="P197" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15487,7 +15487,7 @@
       </c>
       <c r="P198" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15565,7 +15565,7 @@
       </c>
       <c r="P199" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15643,7 +15643,7 @@
       </c>
       <c r="P200" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15717,7 +15717,7 @@
       <c r="O201" t="inlineStr"/>
       <c r="P201" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="P202" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15869,7 +15869,7 @@
       <c r="O203" t="inlineStr"/>
       <c r="P203" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -15947,7 +15947,7 @@
       </c>
       <c r="P204" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16021,7 +16021,7 @@
       <c r="O205" t="inlineStr"/>
       <c r="P205" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16095,7 +16095,7 @@
       <c r="O206" t="inlineStr"/>
       <c r="P206" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16169,7 +16169,7 @@
       <c r="O207" t="inlineStr"/>
       <c r="P207" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16247,7 +16247,7 @@
       </c>
       <c r="P208" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16325,7 +16325,7 @@
       </c>
       <c r="P209" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16403,7 +16403,7 @@
       </c>
       <c r="P210" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16477,7 +16477,7 @@
       <c r="O211" t="inlineStr"/>
       <c r="P211" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16555,7 +16555,7 @@
       </c>
       <c r="P212" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16633,7 +16633,7 @@
       </c>
       <c r="P213" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16707,7 +16707,7 @@
       <c r="O214" t="inlineStr"/>
       <c r="P214" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16781,7 +16781,7 @@
       <c r="O215" t="inlineStr"/>
       <c r="P215" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16855,7 +16855,7 @@
       <c r="O216" t="inlineStr"/>
       <c r="P216" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -16929,7 +16929,7 @@
       <c r="O217" t="inlineStr"/>
       <c r="P217" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17003,7 +17003,7 @@
       <c r="O218" t="inlineStr"/>
       <c r="P218" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17077,7 +17077,7 @@
       <c r="O219" t="inlineStr"/>
       <c r="P219" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17155,7 +17155,7 @@
       </c>
       <c r="P220" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17229,7 +17229,7 @@
       <c r="O221" t="inlineStr"/>
       <c r="P221" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17303,7 +17303,7 @@
       <c r="O222" t="inlineStr"/>
       <c r="P222" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17377,7 +17377,7 @@
       <c r="O223" t="inlineStr"/>
       <c r="P223" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="P224" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17529,7 +17529,7 @@
       <c r="O225" t="inlineStr"/>
       <c r="P225" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17607,7 +17607,7 @@
       </c>
       <c r="P226" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17685,7 +17685,7 @@
       </c>
       <c r="P227" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17761,7 +17761,7 @@
       </c>
       <c r="P228" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17835,7 +17835,7 @@
       <c r="O229" t="inlineStr"/>
       <c r="P229" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17909,7 +17909,7 @@
       <c r="O230" t="inlineStr"/>
       <c r="P230" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -17987,7 +17987,7 @@
       </c>
       <c r="P231" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18065,7 +18065,7 @@
       </c>
       <c r="P232" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18139,7 +18139,7 @@
       <c r="O233" t="inlineStr"/>
       <c r="P233" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18213,7 +18213,7 @@
       <c r="O234" t="inlineStr"/>
       <c r="P234" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18287,7 +18287,7 @@
       <c r="O235" t="inlineStr"/>
       <c r="P235" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18361,7 +18361,7 @@
       <c r="O236" t="inlineStr"/>
       <c r="P236" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18435,7 +18435,7 @@
       <c r="O237" t="inlineStr"/>
       <c r="P237" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18509,7 +18509,7 @@
       <c r="O238" t="inlineStr"/>
       <c r="P238" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18587,7 +18587,7 @@
       </c>
       <c r="P239" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18663,7 +18663,7 @@
       </c>
       <c r="P240" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18735,7 +18735,7 @@
       <c r="O241" t="inlineStr"/>
       <c r="P241" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18809,7 +18809,7 @@
       <c r="O242" t="inlineStr"/>
       <c r="P242" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18881,7 +18881,7 @@
       <c r="O243" t="inlineStr"/>
       <c r="P243" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -18955,7 +18955,7 @@
       <c r="O244" t="inlineStr"/>
       <c r="P244" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19029,7 +19029,7 @@
       <c r="O245" t="inlineStr"/>
       <c r="P245" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19103,7 +19103,7 @@
       <c r="O246" t="inlineStr"/>
       <c r="P246" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19177,7 +19177,7 @@
       <c r="O247" t="inlineStr"/>
       <c r="P247" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19251,7 +19251,7 @@
       <c r="O248" t="inlineStr"/>
       <c r="P248" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19325,7 +19325,7 @@
       <c r="O249" t="inlineStr"/>
       <c r="P249" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19403,7 +19403,7 @@
       </c>
       <c r="P250" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19481,7 +19481,7 @@
       </c>
       <c r="P251" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19555,7 +19555,7 @@
       <c r="O252" t="inlineStr"/>
       <c r="P252" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19633,7 +19633,7 @@
       </c>
       <c r="P253" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19711,7 +19711,7 @@
       </c>
       <c r="P254" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19789,7 +19789,7 @@
       </c>
       <c r="P255" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19861,7 +19861,7 @@
       <c r="O256" t="inlineStr"/>
       <c r="P256" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -19935,7 +19935,7 @@
       <c r="O257" t="inlineStr"/>
       <c r="P257" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20007,7 +20007,7 @@
       <c r="O258" t="inlineStr"/>
       <c r="P258" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20085,7 +20085,7 @@
       </c>
       <c r="P259" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20163,7 +20163,7 @@
       </c>
       <c r="P260" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20241,7 +20241,7 @@
       </c>
       <c r="P261" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20315,7 +20315,7 @@
       <c r="O262" t="inlineStr"/>
       <c r="P262" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20393,7 +20393,7 @@
       </c>
       <c r="P263" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20467,7 +20467,7 @@
       <c r="O264" t="inlineStr"/>
       <c r="P264" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20545,7 +20545,7 @@
       </c>
       <c r="P265" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20619,7 +20619,7 @@
       <c r="O266" t="inlineStr"/>
       <c r="P266" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20697,7 +20697,7 @@
       </c>
       <c r="P267" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20771,7 +20771,7 @@
       <c r="O268" t="inlineStr"/>
       <c r="P268" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20849,7 +20849,7 @@
       </c>
       <c r="P269" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -20927,7 +20927,7 @@
       </c>
       <c r="P270" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21005,7 +21005,7 @@
       </c>
       <c r="P271" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21077,7 +21077,7 @@
       <c r="O272" t="inlineStr"/>
       <c r="P272" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21151,7 +21151,7 @@
       <c r="O273" t="inlineStr"/>
       <c r="P273" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21229,7 +21229,7 @@
       </c>
       <c r="P274" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21307,7 +21307,7 @@
       </c>
       <c r="P275" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21381,7 +21381,7 @@
       <c r="O276" t="inlineStr"/>
       <c r="P276" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21455,7 +21455,7 @@
       <c r="O277" t="inlineStr"/>
       <c r="P277" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21533,7 +21533,7 @@
       </c>
       <c r="P278" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21611,7 +21611,7 @@
       </c>
       <c r="P279" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21689,7 +21689,7 @@
       </c>
       <c r="P280" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21763,7 +21763,7 @@
       <c r="O281" t="inlineStr"/>
       <c r="P281" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21841,7 +21841,7 @@
       </c>
       <c r="P282" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21915,7 +21915,7 @@
       <c r="O283" t="inlineStr"/>
       <c r="P283" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -21989,7 +21989,7 @@
       <c r="O284" t="inlineStr"/>
       <c r="P284" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22067,7 +22067,7 @@
       </c>
       <c r="P285" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22141,7 +22141,7 @@
       <c r="O286" t="inlineStr"/>
       <c r="P286" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22215,7 +22215,7 @@
       <c r="O287" t="inlineStr"/>
       <c r="P287" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22289,7 +22289,7 @@
       <c r="O288" t="inlineStr"/>
       <c r="P288" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22365,7 +22365,7 @@
       </c>
       <c r="P289" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22443,7 +22443,7 @@
       </c>
       <c r="P290" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22521,7 +22521,7 @@
       </c>
       <c r="P291" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22595,7 +22595,7 @@
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22673,7 +22673,7 @@
       </c>
       <c r="P293" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22747,7 +22747,7 @@
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22821,7 +22821,7 @@
       <c r="O295" t="inlineStr"/>
       <c r="P295" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22899,7 +22899,7 @@
       </c>
       <c r="P296" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -22971,7 +22971,7 @@
       <c r="O297" t="inlineStr"/>
       <c r="P297" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23045,7 +23045,7 @@
       <c r="O298" t="inlineStr"/>
       <c r="P298" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23119,7 +23119,7 @@
       <c r="O299" t="inlineStr"/>
       <c r="P299" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23193,7 +23193,7 @@
       <c r="O300" t="inlineStr"/>
       <c r="P300" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23267,7 +23267,7 @@
       <c r="O301" t="inlineStr"/>
       <c r="P301" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23341,7 +23341,7 @@
       <c r="O302" t="inlineStr"/>
       <c r="P302" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23415,7 +23415,7 @@
       <c r="O303" t="inlineStr"/>
       <c r="P303" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23489,7 +23489,7 @@
       <c r="O304" t="inlineStr"/>
       <c r="P304" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23563,7 +23563,7 @@
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23637,7 +23637,7 @@
       <c r="O306" t="inlineStr"/>
       <c r="P306" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23711,7 +23711,7 @@
       <c r="O307" t="inlineStr"/>
       <c r="P307" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23785,7 +23785,7 @@
       <c r="O308" t="inlineStr"/>
       <c r="P308" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23863,7 +23863,7 @@
       </c>
       <c r="P309" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -23937,7 +23937,7 @@
       <c r="O310" t="inlineStr"/>
       <c r="P310" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24011,7 +24011,7 @@
       <c r="O311" t="inlineStr"/>
       <c r="P311" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24085,7 +24085,7 @@
       <c r="O312" t="inlineStr"/>
       <c r="P312" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24163,7 +24163,7 @@
       </c>
       <c r="P313" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24241,7 +24241,7 @@
       </c>
       <c r="P314" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24319,7 +24319,7 @@
       </c>
       <c r="P315" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24393,7 +24393,7 @@
       <c r="O316" t="inlineStr"/>
       <c r="P316" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24465,7 +24465,7 @@
       <c r="O317" t="inlineStr"/>
       <c r="P317" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24543,7 +24543,7 @@
       </c>
       <c r="P318" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24617,7 +24617,7 @@
       <c r="O319" t="inlineStr"/>
       <c r="P319" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24691,7 +24691,7 @@
       <c r="O320" t="inlineStr"/>
       <c r="P320" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24765,7 +24765,7 @@
       <c r="O321" t="inlineStr"/>
       <c r="P321" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24839,7 +24839,7 @@
       <c r="O322" t="inlineStr"/>
       <c r="P322" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24913,7 +24913,7 @@
       <c r="O323" t="inlineStr"/>
       <c r="P323" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -24987,7 +24987,7 @@
       <c r="O324" t="inlineStr"/>
       <c r="P324" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25061,7 +25061,7 @@
       <c r="O325" t="inlineStr"/>
       <c r="P325" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25133,7 +25133,7 @@
       <c r="O326" t="inlineStr"/>
       <c r="P326" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25207,7 +25207,7 @@
       <c r="O327" t="inlineStr"/>
       <c r="P327" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25281,7 +25281,7 @@
       <c r="O328" t="inlineStr"/>
       <c r="P328" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25359,7 +25359,7 @@
       </c>
       <c r="P329" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25437,7 +25437,7 @@
       </c>
       <c r="P330" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25513,7 +25513,7 @@
       </c>
       <c r="P331" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25587,7 +25587,7 @@
       <c r="O332" t="inlineStr"/>
       <c r="P332" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25661,7 +25661,7 @@
       <c r="O333" t="inlineStr"/>
       <c r="P333" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25735,7 +25735,7 @@
       <c r="O334" t="inlineStr"/>
       <c r="P334" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25809,7 +25809,7 @@
       <c r="O335" t="inlineStr"/>
       <c r="P335" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25885,7 +25885,7 @@
       </c>
       <c r="P336" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -25957,7 +25957,7 @@
       <c r="O337" t="inlineStr"/>
       <c r="P337" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26035,7 +26035,7 @@
       </c>
       <c r="P338" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26111,7 +26111,7 @@
       </c>
       <c r="P339" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26185,7 +26185,7 @@
       <c r="O340" t="inlineStr"/>
       <c r="P340" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26257,7 +26257,7 @@
       <c r="O341" t="inlineStr"/>
       <c r="P341" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26335,7 +26335,7 @@
       </c>
       <c r="P342" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26413,7 +26413,7 @@
       </c>
       <c r="P343" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26487,7 +26487,7 @@
       <c r="O344" t="inlineStr"/>
       <c r="P344" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26565,7 +26565,7 @@
       </c>
       <c r="P345" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26637,7 +26637,7 @@
       <c r="O346" t="inlineStr"/>
       <c r="P346" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26711,7 +26711,7 @@
       <c r="O347" t="inlineStr"/>
       <c r="P347" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26785,7 +26785,7 @@
       <c r="O348" t="inlineStr"/>
       <c r="P348" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26863,7 +26863,7 @@
       </c>
       <c r="P349" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -26941,7 +26941,7 @@
       </c>
       <c r="P350" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27015,7 +27015,7 @@
       <c r="O351" t="inlineStr"/>
       <c r="P351" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27093,7 +27093,7 @@
       </c>
       <c r="P352" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27165,7 +27165,7 @@
       <c r="O353" t="inlineStr"/>
       <c r="P353" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27239,7 +27239,7 @@
       <c r="O354" t="inlineStr"/>
       <c r="P354" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27313,7 +27313,7 @@
       <c r="O355" t="inlineStr"/>
       <c r="P355" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27387,7 +27387,7 @@
       <c r="O356" t="inlineStr"/>
       <c r="P356" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27461,7 +27461,7 @@
       <c r="O357" t="inlineStr"/>
       <c r="P357" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27535,7 +27535,7 @@
       <c r="O358" t="inlineStr"/>
       <c r="P358" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27609,7 +27609,7 @@
       <c r="O359" t="inlineStr"/>
       <c r="P359" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27683,7 +27683,7 @@
       <c r="O360" t="inlineStr"/>
       <c r="P360" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27757,7 +27757,7 @@
       <c r="O361" t="inlineStr"/>
       <c r="P361" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27831,7 +27831,7 @@
       <c r="O362" t="inlineStr"/>
       <c r="P362" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27905,7 +27905,7 @@
       <c r="O363" t="inlineStr"/>
       <c r="P363" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -27979,7 +27979,7 @@
       <c r="O364" t="inlineStr"/>
       <c r="P364" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28053,7 +28053,7 @@
       <c r="O365" t="inlineStr"/>
       <c r="P365" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28127,7 +28127,7 @@
       <c r="O366" t="inlineStr"/>
       <c r="P366" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28201,7 +28201,7 @@
       <c r="O367" t="inlineStr"/>
       <c r="P367" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28279,7 +28279,7 @@
       </c>
       <c r="P368" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28353,7 +28353,7 @@
       <c r="O369" t="inlineStr"/>
       <c r="P369" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28429,7 +28429,7 @@
       </c>
       <c r="P370" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28503,7 +28503,7 @@
       <c r="O371" t="inlineStr"/>
       <c r="P371" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28575,7 +28575,7 @@
       <c r="O372" t="inlineStr"/>
       <c r="P372" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28649,7 +28649,7 @@
       <c r="O373" t="inlineStr"/>
       <c r="P373" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28723,7 +28723,7 @@
       <c r="O374" t="inlineStr"/>
       <c r="P374" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28795,7 +28795,7 @@
       <c r="O375" t="inlineStr"/>
       <c r="P375" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28869,7 +28869,7 @@
       <c r="O376" t="inlineStr"/>
       <c r="P376" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -28943,7 +28943,7 @@
       <c r="O377" t="inlineStr"/>
       <c r="P377" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29017,7 +29017,7 @@
       <c r="O378" t="inlineStr"/>
       <c r="P378" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29091,7 +29091,7 @@
       <c r="O379" t="inlineStr"/>
       <c r="P379" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29169,7 +29169,7 @@
       </c>
       <c r="P380" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29245,7 +29245,7 @@
       </c>
       <c r="P381" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29323,7 +29323,7 @@
       </c>
       <c r="P382" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29395,7 +29395,7 @@
       <c r="O383" t="inlineStr"/>
       <c r="P383" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29467,7 +29467,7 @@
       <c r="O384" t="inlineStr"/>
       <c r="P384" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29539,7 +29539,7 @@
       <c r="O385" t="inlineStr"/>
       <c r="P385" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29611,7 +29611,7 @@
       <c r="O386" t="inlineStr"/>
       <c r="P386" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29685,7 +29685,7 @@
       <c r="O387" t="inlineStr"/>
       <c r="P387" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29759,7 +29759,7 @@
       <c r="O388" t="inlineStr"/>
       <c r="P388" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29837,7 +29837,7 @@
       </c>
       <c r="P389" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29913,7 +29913,7 @@
       </c>
       <c r="P390" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>
@@ -29989,7 +29989,7 @@
       </c>
       <c r="P391" t="inlineStr">
         <is>
-          <t>2022-06-21 06:53:08</t>
+          <t>2022-06-21 07:37:36</t>
         </is>
       </c>
     </row>

</xml_diff>